<commit_message>
Commit de Volumen de Tendencias por Dia - Prueba 1
</commit_message>
<xml_diff>
--- a/ReporteDiario/Volumen de tendencias por Dia.xlsx
+++ b/ReporteDiario/Volumen de tendencias por Dia.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>Tendencia</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>#ParoNacional29M</t>
+  </si>
+  <si>
+    <t>#ParoNacional4J</t>
   </si>
 </sst>
 </file>
@@ -381,7 +384,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,6 +432,14 @@
         <v>8126</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>32000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit 8 Archivos - Prueba 2
</commit_message>
<xml_diff>
--- a/ReporteDiario/Volumen de tendencias por Dia.xlsx
+++ b/ReporteDiario/Volumen de tendencias por Dia.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Tendencia</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>#ParoNacional4J</t>
+  </si>
+  <si>
+    <t>#ParoNacional3J</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,6 +443,14 @@
         <v>32000</v>
       </c>
     </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>